<commit_message>
207 adicionar arquivo de metadados atualizado (#208)
* Metadados atualizado
</commit_message>
<xml_diff>
--- a/public/infos/metadados-datasp.xlsx
+++ b/public/infos/metadados-datasp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\855395\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2722F49E-673D-43D0-AACC-E8E446BBC8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5808923-E6B5-471E-AD52-D13199C62E6B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183DC683-7829-4195-B067-F6EE5E3E96AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10125" activeTab="2" xr2:uid="{5C405DEB-DBE8-4978-A59C-3D6D75628EC4}"/>
   </bookViews>
@@ -27,23 +27,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="296">
   <si>
     <t>Indicador resumido</t>
   </si>
@@ -320,639 +309,695 @@
     <t>Ábaco, TCMSP; Censo, IBGE; Elaboração própria</t>
   </si>
   <si>
-    <t>Despesas totais</t>
+    <t>Prestação de Contas Públicas - Orçamento, PMSP</t>
+  </si>
+  <si>
+    <t>População em Risco Hidrológico e Geológico</t>
+  </si>
+  <si>
+    <t>População em risco geológico e
+hidrológico (2025) (hab.)</t>
+  </si>
+  <si>
+    <t>Mede o número de pessoas em risco hidrológico e geológico no munícipio de São Paulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Polígonos representam as áreas de risco de deslizamento, solapamento, enchentes e inundações em assentamentos precários, especialmente aqueles localizados em encostas ou margens de córregos. A definição de área de risco encontra-se no glossário.</t>
+  </si>
+  <si>
+    <t>População em risco hidrológico + população em risco geológico</t>
+  </si>
+  <si>
+    <t>Censo Demográfico, IBGE,
+GeoSampa/Elaboração própria</t>
+  </si>
+  <si>
+    <t>2022 e 2025</t>
+  </si>
+  <si>
+    <t>População em Risco Hidrológico</t>
+  </si>
+  <si>
+    <t>População em risco hidrológico (2025) (hab.)</t>
+  </si>
+  <si>
+    <t>Mede o número de pessoas em risco hidrológico no munícipio de São Paulo</t>
+  </si>
+  <si>
+    <t>Polígonos representam as áreas de risco de  enchentes e inundações em assentamentos precários, especialmente aqueles localizados em margens de córregos. A definição de área de risco encontra-se no glossário.</t>
+  </si>
+  <si>
+    <t>População em risco hidrológico</t>
+  </si>
+  <si>
+    <t>População em Risco Geológico</t>
+  </si>
+  <si>
+    <t>Mede o número de pessoas em risco geológico no munícipio de São Paulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Polígonos representam as áreas de risco de deslizamento e solapamento em assentamentos precários, especialmente aqueles localizados em encostas ou margens de córregos. A definição de área de risco encontra-se no glossário.</t>
+  </si>
+  <si>
+    <t>População em risco geológico</t>
+  </si>
+  <si>
+    <t>População em risco geológico e
+hidrológico (2025) (%)</t>
+  </si>
+  <si>
+    <t>Mede o percentual de pessoas em risco hidrológico ou geológico no munícipio de São Paulo</t>
+  </si>
+  <si>
+    <t>Polígonos representam as áreas de risco de deslizamento, solapamento, enchentes e inundações em assentamentos precários, especialmente aqueles localizados em encostas ou margens de córregos. A definição de área encontra-se no glossário.</t>
+  </si>
+  <si>
+    <t>Total da população em risco hidrológico e geológico ÷ Total da população</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Censo Demográfico, IBGE,
+GeoSampa </t>
+  </si>
+  <si>
+    <t>População em hidrológico (2025) (%)</t>
+  </si>
+  <si>
+    <t>Mede o percentual de pessoas em risco hidrológico no munícipio de São Paulo</t>
+  </si>
+  <si>
+    <t>Total da população em risco hidrológico ÷ Total da população</t>
+  </si>
+  <si>
+    <t>População em geológico (2025) (%)</t>
+  </si>
+  <si>
+    <t>Total da população em risco geológico ÷ Total da população</t>
+  </si>
+  <si>
+    <t>Mapa Geológico Simplificado</t>
+  </si>
+  <si>
+    <t>Mapa Geológico Simplificado do Município de São Paulo</t>
+  </si>
+  <si>
+    <t>O Mapa geológico simplificado do município de São Paulo foi elaborado a partir do Mapa Geológico de São Paulo (GeoSampa), agrupando as unidades litológicas originais em três classes principais por idade geológica: sedimentos quaternários (planícies aluviais), sedimentos terciários da Bacia de São Paulo e rochas pré-cambrianas (unidades metamórficas e ígneas). Cada classe foi representada por uma cor específica (amarelo, abóbora e rosado, respectivamente), visando facilitar a leitura espacial e a correlação com as áreas de risco.</t>
+  </si>
+  <si>
+    <t>A base utilizada foi o Mapa Geológico de São Paulo (GeoSampa), com classes reagrupadas em três grandes classes para fins de visualização no painel, seguindo lógica cronoestratigráfica. A primeira corresponde aos Sedimentos Quaternários (amarelo), que representam depósitos aluviais recentes vinculados a planícies fluviais. A segunda reúne os Sedimentos Terciários (laranja/abóbora), relacionados às formações da Bacia de São Paulo, compostas por lamitos arenosos, arenitos, siltitos, argilitos e conglomerados. Por fim, destacam-se as Rochas Pré-Cambrianas (rosado), abrangendo unidades metamórficas e ígneas, como metacarbonatos, filitos, xistos, quartzitos, gnaisses, migmatitos, granitos e granitoides. Essa simplificação facilita a leitura do mapa e a interpretação visual, mantendo a representatividade geológica essencial para análises urbanas e ambientais.</t>
+  </si>
+  <si>
+    <t>Não aplicável.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GeoSampa/Elaboração própria </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 e 2025 </t>
+  </si>
+  <si>
+    <t>Valores Liquidados Programa 3008</t>
+  </si>
+  <si>
+    <t>Despesas em Gestão dos Riscos e Promoção da Resiliência a Desastres e Eventos Críticos (2024) (R$)</t>
+  </si>
+  <si>
+    <t>Execução orçamentária liquidada do Programa 3008 – Gestão dos Riscos e Promoção da Resiliência a Desastres e Eventos Críticos, territorializada por Subprefeitura no município de São Paulo.</t>
+  </si>
+  <si>
+    <t>Valores pagos (liquidados) em 2024, referentes aos projetos-atividades do Programa 3008.</t>
+  </si>
+  <si>
+    <t>Soma dos valores liquidados por projeto-atividade (2112, 2367, 4901, 5013), agregados pela Subprefeitura da unidade executora no ano de 2024</t>
+  </si>
+  <si>
+    <t>Secretaria Municipal da Fazenda (PMSP)</t>
+  </si>
+  <si>
+    <t>Auxílio Aluguel</t>
+  </si>
+  <si>
+    <t>11.01.08 - Total de famílias beneficiárias de Auxílio Aluguel por ano (familias)</t>
+  </si>
+  <si>
+    <t>Mede o número de famílias beneficiárias de Auxílio Aluguel em cada ano usando como referência o mês de dezembro</t>
+  </si>
+  <si>
+    <t>O número de famílias beneficiárias de Auxílio Aluguél nos meses de dezembro permite uma comparação anual do fluxo de benefícios concedidos ao longo da série histórica.</t>
+  </si>
+  <si>
+    <t>Número de famílias beneficiárias de Auxílio Aluguel</t>
+  </si>
+  <si>
+    <t>ObservaSampa (HabitaSampa; Secretaria Municipal de Habitação (SEHAB)).</t>
+  </si>
+  <si>
+    <t>Auxílio Aluguel - Por Situação de Risco e Emergência</t>
+  </si>
+  <si>
+    <t>01.05.02 - Número de famílias em atendimento habitacional provisório (Auxílio Aluguel) por situação de risco e emergência (familias)</t>
+  </si>
+  <si>
+    <t>Mede a quantidade total de famílias em atendimento habitacional provisório pela SEHAB em um determinado período, que tenha como motivo da inclusão no benefício uma situação emergencial ou situação de risco, em um determinado período.</t>
+  </si>
+  <si>
+    <t>Número de famílias em atendimento habitacional provisório (Auxílio Aluguel) por situação de risco e emergência</t>
+  </si>
+  <si>
+    <t>ObservaSampa (Sistema Municipal de Informações Habitacionais (Habitasampa)/Secretaria Municipal de Habitação (SEHAB)/Departamento de Planejamento Habitacional (DEPLAN)).</t>
+  </si>
+  <si>
+    <t>Mapa de Parques Municipais e Estaduais</t>
+  </si>
+  <si>
+    <t>Área de Parque (%) por Subprefeitura (2024)</t>
+  </si>
+  <si>
+    <t>Mede a proporção da área ocupada por parques (municipais e estaduais) em relação à área total de cada subprefeitura no município de São Paulo.</t>
+  </si>
+  <si>
+    <t>Os polígonos de parques foram obtidos do GeoSampa (camada de Parques Existentes) e cruzados com os limites territoriais oficiais de cada subprefeitura. O indicador expressa o peso relativo das áreas de parques dentro de cada unidade administrativa, permitindo identificar diferenças na cobertura verde destinada a lazer e conservação ambiental.</t>
+  </si>
+  <si>
+    <t>Área de Parques na Subprefeitura (m²) ÷ Área Total da Subprefeitura (m²) × 100</t>
+  </si>
+  <si>
+    <t>GeoSampa</t>
+  </si>
+  <si>
+    <t>Parques, Área Permeável</t>
+  </si>
+  <si>
+    <t>Parques Novos e Requalificados e Áreas Permeáveis (2024) (%)</t>
+  </si>
+  <si>
+    <t>Mede a proporção de áreas permeáveis (incluindo parques, beiras de estrada e demais áreas não impermeabilizadas) em relação à área terrestre total do município, excluídas áreas marinhas sob jurisdição da cidade.</t>
+  </si>
+  <si>
+    <t>Área permeável total ÷ Área terrestre total da cidade × 100</t>
+  </si>
+  <si>
+    <t>Biosampa 2023 / Secretaria do Verde e do Meio Ambiente (SVMA-PMSP).</t>
+  </si>
+  <si>
+    <t>Valores Liquidados</t>
+  </si>
+  <si>
+    <t>Valores Liquidados (2024) - R$308.579.562,86 (Projeto 1702 + 1703) (R$)</t>
+  </si>
+  <si>
+    <t>Mede o valor liquidado do orçamento destinado por subprefeitura aos projetos e atividades 1702 (Construção e Implantação de Parques Urbanos e Lineares) e 1703 (Ampliação, Reforma e Requalificação de Parques Urbanos e Lineares).</t>
+  </si>
+  <si>
+    <t>Portal de Prestação de Contas Públicas / Secretaria Municipal da Fazenda (PMSP).</t>
+  </si>
+  <si>
+    <t>Déficit habitacional Municipal</t>
+  </si>
+  <si>
+    <t>11.01.01 - Déficit habitacional em relação ao total de domicílios (UN)</t>
+  </si>
+  <si>
+    <t>Não Disponível</t>
+  </si>
+  <si>
+    <t>São características principais do déficit habitacional, de acordo com o IPEA, a reposição de estoque e o incremento de estoque. A reposição de estoque contempla a necessidade de repor as habitações em função da sua precariedade e desgaste de uso. O incremento de estoque refere-se a demanda por novas moradias decorrente de: (a) coabitação forçada (aquela na qual a família convivente deseja constituir novo domicílio, mas não possui condições necessárias para tal); (b) famílias que residem em imóveis locados, com valores que comprometem mais de 30% da renda familiar; e (c) o adensamento excessivo em imóveis locados.</t>
+  </si>
+  <si>
+    <t>Número de domicílios com déficit ÷ Domicílios particulares permanentes × 100</t>
+  </si>
+  <si>
+    <t>ObservaSampa</t>
+  </si>
+  <si>
+    <t>Domicílios não ocupados</t>
+  </si>
+  <si>
+    <t>Domicílios não ocupados (UN)</t>
+  </si>
+  <si>
+    <t>Indica o número total de unidades habitacionais
+particulares existentes no território que, no momento da coleta censitária, não estavam sendo utilizadas como moradia principal.</t>
+  </si>
+  <si>
+    <t>São considerados domicílios não ocupados aqueles que, no momento da coleta do Censo Demográfico, não possuíam uso residencial ativo — incluindo tanto unidades vagas, sem moradores presentes, quanto domicílios ocupados sem entrevista, onde havia moradores mas a entrevista não foi realizada (por ausência ou recusa) — e domicílios de uso ocasional, utilizados apenas temporariamente para fins de descanso ou lazer.</t>
+  </si>
+  <si>
+    <t>Total de domicílios – Total de domicílios particulares permanentes ocupados</t>
+  </si>
+  <si>
+    <t>Censo Demográfico – Instituto Brasileiro de Geografia e Estatística (IBGE)/Elaboração própria</t>
+  </si>
+  <si>
+    <t>Domicílios não ocupados (%)</t>
+  </si>
+  <si>
+    <t>Indica o percentual em relação a subprefeitura de unidades habitacionais
+particulares existentes no território que, no momento da coleta censitária, não estavam sendo utilizadas como moradia principal.</t>
+  </si>
+  <si>
+    <t>Total de domicilios não ocupados ÷ Total de domicilios</t>
+  </si>
+  <si>
+    <t>Domicílios em Favelas</t>
+  </si>
+  <si>
+    <t>Número total de domicílios Favelas (UN)</t>
+  </si>
+  <si>
+    <t>Estimativa dos domicílios em favelas existentes em São Paulo</t>
+  </si>
+  <si>
+    <t>Número de domicilios em favela</t>
+  </si>
+  <si>
+    <t>ObservaSampa (Sistema Municipal de Informações Habitacionais (Habitasampa)/Secretaria Municipal de Habitação (SEHAB)</t>
+  </si>
+  <si>
+    <t>Unidades habitacionais entregues</t>
+  </si>
+  <si>
+    <t>Indicador 11.01.03 - Número de Unidades Habitacionais entregues (por meio de programas habitacionais e parcerias firmadas) (UN)</t>
+  </si>
+  <si>
+    <t>Apresenta a quantidade de Unidades Habitacionais entregues (por meio de programas habitacionais e parcerias firmadas).</t>
+  </si>
+  <si>
+    <t>Um elevado valor indica maior quantidade de
+Unidades Habitacionais entregues, o que represente um fortalecimento das políticas de moradia.</t>
+  </si>
+  <si>
+    <t>Unidades Habitacionais entregues (por meio de programas habitacionais e parcerias firmadas)</t>
+  </si>
+  <si>
+    <t>ObservaSampa (Sistema Municipal de
+Informações Habitacionais (Habitasampa)/Secretaria Municipal de Habitação (SEHAB)</t>
+  </si>
+  <si>
+    <t>Unidades habitacionais entregues e contratadas</t>
+  </si>
+  <si>
+    <t>Meta 12 do Programa de Metas 2021-2024 - Unidades habitacionais entregues e contratadas (UN)</t>
+  </si>
+  <si>
+    <t>O indicador considera as unidades entregues e contratadas por meio dos programas:
+Pode Entrar, Operações Urbanas Consorciadas, Parcerias Público-Privadas, Minha Casa Minha Vida, Casa Verde Amarela, Locação Social, Convênios e outros programas habitacionais.</t>
+  </si>
+  <si>
+    <t>Promover o acesso à moradia, à urbanização e à regularização fundiária para famílias de baixa renda.</t>
+  </si>
+  <si>
+    <t>Somatória do número de unidades habitacionais de interesse social, entregues e contratadas pelo poder público.</t>
+  </si>
+  <si>
+    <t>Programa de Metas – PMSP</t>
+  </si>
+  <si>
+    <t>Regularização fundiária urbana</t>
+  </si>
+  <si>
+    <t>Indicador 11.01.02 - Número de famílias beneficiadas por procedimentos de regularização fundiária em núcleos urbanos informais (familias)</t>
+  </si>
+  <si>
+    <t>Apresenta o número de famílias beneficiadas
+por procedimentos de regularização fundiária.</t>
+  </si>
+  <si>
+    <t>Um valor elevado desse número representa maior quantidades de famílias que usufruiram da regularização fundiária em núcleos urbanos informais.</t>
+  </si>
+  <si>
+    <t>Número de famílias beneficiadas por procedimentos de regularização fundiária em assentamentos precários</t>
+  </si>
+  <si>
+    <t>ObservaSampa/Secretaria Municipal de Habitação (SEHAB)</t>
+  </si>
+  <si>
+    <t>Obras em assentamentos precários</t>
+  </si>
+  <si>
+    <t>Indicador 11.01.06 - Número de famílias beneficiadas com obras de urbanização de assentamentos precários (familias)</t>
+  </si>
+  <si>
+    <t>Trata-se de famílias beneficiadas com as obras já iniciadas nesses territórios</t>
+  </si>
+  <si>
+    <t>Um valor elevado desse número representa maior quantidades de famílias que usufruiram das obras de urbanização de assentamentos precários.</t>
+  </si>
+  <si>
+    <t>Número de famílias beneficiadas com obras de urbanização de assentamentos precários em andamento</t>
+  </si>
+  <si>
+    <t>Orçado inicial</t>
+  </si>
+  <si>
+    <t>Valor orçado em reais</t>
+  </si>
+  <si>
+    <t>Valor orçamentário fixado pela Lei Orçamentária Anual. O valor aparece em relação a todo o orçamento muncipal, ou ao orçamento de cada função ou de cada projeto atividade.</t>
+  </si>
+  <si>
+    <t>É o valor aprovado na Lei Orçamentária Anual (LOA) no começo do ano. Representa a previsão oficial de quanto a prefeitura pretendia gastar e arrecadar em cada área antes de qualquer mudança. Serve como ponto de partida para acompanhar a execução orçamentária.</t>
+  </si>
+  <si>
+    <t>Valor orçado</t>
+  </si>
+  <si>
+    <t>Orçado atualizado</t>
+  </si>
+  <si>
+    <t>Valor atualizado em reais</t>
+  </si>
+  <si>
+    <t>Valor orçamentário vigente após as alterações ocorridas durante a execução orçamentária, considerando créditos adicionais (suplementações, anulações e remanejamentos)</t>
+  </si>
+  <si>
+    <t>É o orçamento inicial ajustado pelas modificações legais e infralegais ocorridas ao longo do exercício, refletindo a dotação disponível para execução.</t>
+  </si>
+  <si>
+    <t>Valor orçado + suplementação líquida</t>
+  </si>
+  <si>
+    <t>Variação em relação ao orçamento inicial (R$)</t>
+  </si>
+  <si>
+    <t>Suplementação líquida em reais</t>
+  </si>
+  <si>
+    <t>Indica o valor nominal da suplementação líquida. O valor aparece em relação a todo o orçamento muncipal, ou ao orçamento de cada função ou de cada projeto atividade.</t>
+  </si>
+  <si>
+    <t>Representa o aumento de recursos por crédito adicional, para reforçar as dotações que já constam na lei orçamentária, descontando-se as deduções.</t>
+  </si>
+  <si>
+    <t>Suplementação líquida</t>
+  </si>
+  <si>
+    <t>Variação em relação ao orçamento inicial (%)</t>
+  </si>
+  <si>
+    <t>Suplementação líquida em relação ao orçamento inicial</t>
+  </si>
+  <si>
+    <t>Indica o valor percentual da suplementação líquida em relação ao valor orçado inicial. O valor aparece em relação a todo o orçamento muncipal, ou ao orçamento de cada função ou de cada projeto atividade.</t>
+  </si>
+  <si>
+    <t>Representa o aumento de recursos por crédito adicional, para reforçar as dotações que já constam na lei orçamentária, descontando-se as deduções. O valor é apresentado em formato percentual, relativo ao valor orçado inicial do escopo analisado.</t>
+  </si>
+  <si>
+    <t>Suplementação líquida ÷ Orçamento inicial × 100</t>
+  </si>
+  <si>
+    <t>Variação da participação relativa no orçamento (%)</t>
+  </si>
+  <si>
+    <t>Variação da participação relativa no orçamento</t>
+  </si>
+  <si>
+    <t>Valor percentual da variação entre a participação relativa de cada função de governo no orçamento municipal.</t>
+  </si>
+  <si>
+    <t>Representa a variação da importância relativa de cada função de governo dentro do orçamento municipal</t>
+  </si>
+  <si>
+    <t>[(Orçamento atualizado da função ÷ Orçamento atualizado do Município) - (Orçamento inicial da função ÷ Orçamento inicial do Município)] ÷ (Orçamento inicial da função ÷ Orçamento inicial do Município)</t>
+  </si>
+  <si>
+    <t>Prestação de Contas Públicas - Orçamento, PMSP; Elaboração Própria</t>
+  </si>
+  <si>
+    <t>Liquidado</t>
+  </si>
+  <si>
+    <t>Valor liquidado em reais</t>
+  </si>
+  <si>
+    <t>Somatório de todas as Notas de Liquidação e Pagamento emitidas. O valor aparece em relação a todo o orçamento muncipal, ou ao orçamento de cada função ou de cada projeto atividade.</t>
+  </si>
+  <si>
+    <t>Valor liquidado</t>
+  </si>
+  <si>
+    <t>Mortalidade por Causas Evitáveis</t>
+  </si>
+  <si>
+    <t>Taxa de Mortalidade por Causas Evitáveis / 100 mil hab.</t>
+  </si>
+  <si>
+    <t>Indica a quantidade relativa de mortes que ocorrem por causas para as quais existe prevenção conhecida e eficaz</t>
+  </si>
+  <si>
+    <t>Representa a quantidade de mortes que poderiam ser evitadas se o método de prevenção (p. ex. vacinas) ou  ações educativas e terapêuticas contra fatores de risco (p. ex. obesidade, hipertensão arterial, diabetes mellitus, etc...) estivessem disponíveis na fase evitável da doença. Este indicador tem relação direta com o investimento de recursos públicos na Atenção Primária em Saúde.</t>
+  </si>
+  <si>
+    <t>SIM - Sistema de Informação sobre Mortalidade; IBGE -  Instituto Bbrasileiro de Geografia e Estatística</t>
+  </si>
+  <si>
+    <t>Mortalidade por Causas Tratáveis</t>
+  </si>
+  <si>
+    <t>Taxa de Mortalidade por Causas Tratáveis / 100 mil hab.</t>
+  </si>
+  <si>
+    <t>Indica a quantidade relativa de mortes que ocorrem por causas para as quais existem tratamentos conhecidos e eficazes.</t>
+  </si>
+  <si>
+    <t>Representa a quantidade de mortes que poderiam não acontecer se os métodos de diagnóstico precoce e tratamento oportuno (p. ex. Câncer de Colo Uterino, Diabetes Mellitus, etc...)  fossem realizados no momento oportuno do desenvolvimento da doença. Este indicador tem relação direta com o investimento de recursos públicos na Atenção Especializada e Hospittalar.</t>
+  </si>
+  <si>
+    <t>Mortalidade por Causas Evitáveis/Tratáveis</t>
+  </si>
+  <si>
+    <t>Taxa de Mortalidade por Causas Evitáveis/Tratáveis / 100 mil hab.</t>
+  </si>
+  <si>
+    <t>Indica a somatória das quantidades relativas de mortes que ocorrem por causas para as quais existe prevenção conhecida e eficaz e por cacusas para as quais existem tratamentos conhecidos e eficazes.</t>
+  </si>
+  <si>
+    <t>Este indicador elimina a quantidade relativa de mortes por causas que independem da administração pública (p. ex. doenças genéticas, congênitas, hereditárias, etc...) e evidencia a quantidade relativa de mortes que em tese poderia ser impactada por ações do investimento público em Saúde.</t>
+  </si>
+  <si>
+    <t>Despesas "per capita" em Atenção Primária</t>
+  </si>
+  <si>
+    <t>Despesas "per capita" em Atenção Primária e Vigilância Sanitária / hab.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indica o montante do investimento público em ações de promoção da saúde e prevenção de doenças. </t>
+  </si>
+  <si>
+    <t>Representa o volume de investimento de recursos públicos em saúde ANTES do surgimento das doenças.</t>
+  </si>
+  <si>
+    <t>IBGE -  Instituto Bbrasileiro de Geografia e Estatística; SIOPS - Sistema de Informações sobre Orçamentos Públicos em Saúde; FNS - Fundo Nacional de Saúde</t>
+  </si>
+  <si>
+    <t>Despesas "per capita" em Atenção Especializada</t>
+  </si>
+  <si>
+    <t>Despesas "per capita" em Atenção Especializada e Suporte Profilático Terapêutico / hab</t>
+  </si>
+  <si>
+    <t>Indica o montante do investimento de recursos públicos em ações curativas e de reabilitação</t>
+  </si>
+  <si>
+    <t>Representa o volume de investimento de recursos públicos em tratamento, DEPOIS que a doença já se instalou, e necessita de atendimento de urgência (UPAs) e de tratamento hospitalar especializado.</t>
+  </si>
+  <si>
+    <t>Leitos de Internação</t>
+  </si>
+  <si>
+    <t>Leitos de Internação / 100 mil hab.</t>
+  </si>
+  <si>
+    <t>Representa o volume de investimento de recursos públicos em tratamento, DEPOIS que a doença já se instalou, e necessita de tratamento hospitalar especializado.</t>
+  </si>
+  <si>
+    <t>IBGE -  Instituto Bbrasileiro de Geografia e Estatística; CNES - Cadastro Nacional de Estabelecimentos de Saúde</t>
+  </si>
+  <si>
+    <t>Leitos Complementares</t>
+  </si>
+  <si>
+    <t>Leitos Complementares / 100 mil hab.</t>
+  </si>
+  <si>
+    <t>Indica o montante do investimento de recursos públicos em atendimento a situações de urgência e emergências, como leitos de Salas de Emergência  e de Salas de Observação em Pronto Socorros e UPAs.</t>
+  </si>
+  <si>
+    <t>Representa o volume de investimento de recursos públicos em Salas de Emergência  e Salas de Observação em Pronto Socorros e UPAs,  onde o risco de morte é importante ou iminente.</t>
+  </si>
+  <si>
+    <t>Leitos de UTI</t>
+  </si>
+  <si>
+    <t>Equipamentos respiradores e ventiladores / 100 mil hab.</t>
+  </si>
+  <si>
+    <t>Indica o montante do investimento de recursos públicos em atendimento a situações de alta gravidade, com allrisco de morte.</t>
+  </si>
+  <si>
+    <t>Representa o volume de investimento de recursos públicos em equipamentos de de atendimento a situações de alto risco de morte iminente. Em muitas situações este equipamento é usado para tratar  eventos de alta gravidade que poderiam ter sido evitados com programas eficazes de promoção da saúde e prevenção de doenças.</t>
+  </si>
+  <si>
+    <t>População</t>
+  </si>
+  <si>
+    <t>População (x 1 mil hab.)</t>
+  </si>
+  <si>
+    <t>Indica a qauntidade de pessoas que habitam o território do município</t>
+  </si>
+  <si>
+    <t>Representa um indicadoo importante para dimensionar corretamente a importância e o impacto dos demais indicadores deste conjunto.</t>
+  </si>
+  <si>
+    <t>Número absoluto de habitantes (em milhares)</t>
+  </si>
+  <si>
+    <t>IBGE -  Instituto Bbrasileiro de Geografia e Estatística</t>
+  </si>
+  <si>
+    <t>Área</t>
+  </si>
+  <si>
+    <t>Indica a dimensão do território considerado na anãlise dos investimentos de recursos públicos</t>
+  </si>
+  <si>
+    <t>Número absoluto de km2 da área municipal</t>
+  </si>
+  <si>
+    <t>Densidade Demográfica</t>
+  </si>
+  <si>
+    <t>Indica a quantidade de pessoas por unidade de território</t>
+  </si>
+  <si>
+    <t>Idosos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porcentagem de Idosos (%) </t>
+  </si>
+  <si>
+    <t>Indica a proporção de idosos na população geral do território</t>
+  </si>
+  <si>
+    <t>Representa um recorte importante do panorama da necessidade de açoes de saúde na população. A porcentagem de idosos indica a demanda de ações de saúde preventivas e curativas a longo prazo, impactando a destinação  de recursos públicos.</t>
+  </si>
+  <si>
+    <t>PIB "per capita"</t>
+  </si>
+  <si>
+    <t>Produto Interno Bruto "per capita"</t>
+  </si>
+  <si>
+    <t>Indica a quantidade de recursos públicos que estará disponível para investimento nas nececssidades sociais.</t>
+  </si>
+  <si>
+    <t>Representa o limite dos recursos disponíveis para investimento nas necessidades sociais</t>
+  </si>
+  <si>
+    <t>Usuários de Planos de Saúde</t>
+  </si>
+  <si>
+    <t>Porcentagem de Usuários de Planos de Saúde Privados (%)</t>
+  </si>
+  <si>
+    <t>Indica  a quantidade relativa de habitantes que são usuário de serviçoos de saúde privados, independentes dos recursos públicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Representa a quantidade relativa da população que utiliza recursos privados para a assistência à saúde. É importante notar que essa parcela da população não consome recursos do SUS na Assistência Especializada Ambulatorial e Hospitalar, mas vai recorrer ao SUS nas situaçãoes de maior custo, como tratamento de câncer e transplantes de órgãos. </t>
+  </si>
+  <si>
+    <t>ANS - Agência Nacional de Saúde Suplementar</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Total de despesas liquidadas na função de governo Saúde em reais </t>
+      <t>Área (km</t>
     </r>
     <r>
       <rPr>
-        <i/>
-        <sz val="12"/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>per capita</t>
-    </r>
-  </si>
-  <si>
-    <t>Somatório de todas as Notas de Liquidação e Pagamento emitidas na função de governo Saúde. O valor aparece em relação a todo o orçamento muncipal, ao orçamento de cada subfunção, de programa ou de Subprefeitura.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Valor liquidado na função Saúde </t>
+      <t>2</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>÷</t>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Densidade Demográfica (hab./km</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> habitantes</t>
-    </r>
-  </si>
-  <si>
-    <t>Prestação de Contas Públicas - Orçamento, PMSP</t>
-  </si>
-  <si>
-    <t>Qtd. Consultas</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Total de consultas </t>
+      <t>2</t>
     </r>
     <r>
       <rPr>
-        <i/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>per capita</t>
+      <t>)</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> na rede pública de saúde </t>
-    </r>
-  </si>
-  <si>
-    <t>Contagem de todas as consultas na rede pública de saúde do município. O valor é exibido em relação a todo o município, a cada Subprefeitura, nível de atenção, categoria ou subcategoria de consulta.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Contagem de consultas </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>÷</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> habitantes</t>
-    </r>
-  </si>
-  <si>
-    <t>Boletim Saúde em Dados, PMSP</t>
-  </si>
-  <si>
-    <t>Qtd. Óbitos</t>
-  </si>
-  <si>
-    <t>Taxa de mortalidade (100.000 habitantes)</t>
-  </si>
-  <si>
-    <t>Contagem de todos os óbitos de habitantes do município de São Paulo dividido por 100.000 habitantes. O valor é exibido em relação a todo o município, às categorias tratável/evitátvel ou a cada Subprefeitura.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Óbitos </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>÷</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> população residente </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>×</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 100.000</t>
-    </r>
-  </si>
-  <si>
-    <t>TabNet, PMSP; Elaboração própria</t>
-  </si>
-  <si>
-    <t>Qtd. Leitos</t>
-  </si>
-  <si>
-    <t>Leitos por 100.000 habitantes</t>
-  </si>
-  <si>
-    <t>Contagem de todos os leitos SUS do município de São Paulo dividido por 100.000 habitantes. O valor é exibido em relação a todo o município, às categorias complementar/internação ou a cada Subprefeitura.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Leitos </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>÷</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> população residente </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>×</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 100.000</t>
-    </r>
-  </si>
-  <si>
-    <t>TabNet, PMSP</t>
-  </si>
-  <si>
-    <t>População em Risco Hidrológico e Geológico</t>
-  </si>
-  <si>
-    <t>População em risco geológico e
-hidrológico (2025) (hab.)</t>
-  </si>
-  <si>
-    <t>Mede o número de pessoas em risco hidrológico e geológico no munícipio de São Paulo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Polígonos representam as áreas de risco de deslizamento, solapamento, enchentes e inundações em assentamentos precários, especialmente aqueles localizados em encostas ou margens de córregos. A definição de área de risco encontra-se no glossário.</t>
-  </si>
-  <si>
-    <t>População em risco hidrológico + população em risco geológico</t>
-  </si>
-  <si>
-    <t>Censo Demográfico, IBGE,
-GeoSampa/Elaboração própria</t>
-  </si>
-  <si>
-    <t>2022 e 2025</t>
-  </si>
-  <si>
-    <t>População em Risco Hidrológico</t>
-  </si>
-  <si>
-    <t>População em risco hidrológico (2025) (hab.)</t>
-  </si>
-  <si>
-    <t>Mede o número de pessoas em risco hidrológico no munícipio de São Paulo</t>
-  </si>
-  <si>
-    <t>Polígonos representam as áreas de risco de  enchentes e inundações em assentamentos precários, especialmente aqueles localizados em margens de córregos. A definição de área de risco encontra-se no glossário.</t>
-  </si>
-  <si>
-    <t>População em risco hidrológico</t>
-  </si>
-  <si>
-    <t>População em Risco Geológico</t>
-  </si>
-  <si>
-    <t>Mede o número de pessoas em risco geológico no munícipio de São Paulo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Polígonos representam as áreas de risco de deslizamento e solapamento em assentamentos precários, especialmente aqueles localizados em encostas ou margens de córregos. A definição de área de risco encontra-se no glossário.</t>
-  </si>
-  <si>
-    <t>População em risco geológico</t>
-  </si>
-  <si>
-    <t>População em risco geológico e
-hidrológico (2025) (%)</t>
-  </si>
-  <si>
-    <t>Mede o percentual de pessoas em risco hidrológico ou geológico no munícipio de São Paulo</t>
-  </si>
-  <si>
-    <t>Polígonos representam as áreas de risco de deslizamento, solapamento, enchentes e inundações em assentamentos precários, especialmente aqueles localizados em encostas ou margens de córregos. A definição de área encontra-se no glossário.</t>
-  </si>
-  <si>
-    <t>Total da população em risco hidrológico e geológico ÷ Total da população</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Censo Demográfico, IBGE,
-GeoSampa </t>
-  </si>
-  <si>
-    <t>População em hidrológico (2025) (%)</t>
-  </si>
-  <si>
-    <t>Mede o percentual de pessoas em risco hidrológico no munícipio de São Paulo</t>
-  </si>
-  <si>
-    <t>Total da população em risco hidrológico ÷ Total da população</t>
-  </si>
-  <si>
-    <t>População em geológico (2025) (%)</t>
-  </si>
-  <si>
-    <t>Total da população em risco geológico ÷ Total da população</t>
-  </si>
-  <si>
-    <t>Mapa Geológico Simplificado</t>
-  </si>
-  <si>
-    <t>Mapa Geológico Simplificado do Município de São Paulo</t>
-  </si>
-  <si>
-    <t>O Mapa geológico simplificado do município de São Paulo foi elaborado a partir do Mapa Geológico de São Paulo (GeoSampa), agrupando as unidades litológicas originais em três classes principais por idade geológica: sedimentos quaternários (planícies aluviais), sedimentos terciários da Bacia de São Paulo e rochas pré-cambrianas (unidades metamórficas e ígneas). Cada classe foi representada por uma cor específica (amarelo, abóbora e rosado, respectivamente), visando facilitar a leitura espacial e a correlação com as áreas de risco.</t>
-  </si>
-  <si>
-    <t>A base utilizada foi o Mapa Geológico de São Paulo (GeoSampa), com classes reagrupadas em três grandes classes para fins de visualização no painel, seguindo lógica cronoestratigráfica. A primeira corresponde aos Sedimentos Quaternários (amarelo), que representam depósitos aluviais recentes vinculados a planícies fluviais. A segunda reúne os Sedimentos Terciários (laranja/abóbora), relacionados às formações da Bacia de São Paulo, compostas por lamitos arenosos, arenitos, siltitos, argilitos e conglomerados. Por fim, destacam-se as Rochas Pré-Cambrianas (rosado), abrangendo unidades metamórficas e ígneas, como metacarbonatos, filitos, xistos, quartzitos, gnaisses, migmatitos, granitos e granitoides. Essa simplificação facilita a leitura do mapa e a interpretação visual, mantendo a representatividade geológica essencial para análises urbanas e ambientais.</t>
-  </si>
-  <si>
-    <t>Não aplicável.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GeoSampa/Elaboração própria </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 e 2025 </t>
-  </si>
-  <si>
-    <t>Valores Liquidados Programa 3008</t>
-  </si>
-  <si>
-    <t>Despesas em Gestão dos Riscos e Promoção da Resiliência a Desastres e Eventos Críticos (2024) (R$)</t>
-  </si>
-  <si>
-    <t>Execução orçamentária liquidada do Programa 3008 – Gestão dos Riscos e Promoção da Resiliência a Desastres e Eventos Críticos, territorializada por Subprefeitura no município de São Paulo.</t>
-  </si>
-  <si>
-    <t>Valores pagos (liquidados) em 2024, referentes aos projetos-atividades do Programa 3008.</t>
-  </si>
-  <si>
-    <t>Soma dos valores liquidados por projeto-atividade (2112, 2367, 4901, 5013), agregados pela Subprefeitura da unidade executora no ano de 2024</t>
-  </si>
-  <si>
-    <t>Secretaria Municipal da Fazenda (PMSP)</t>
-  </si>
-  <si>
-    <t>Auxílio Aluguel</t>
-  </si>
-  <si>
-    <t>11.01.08 - Total de famílias beneficiárias de Auxílio Aluguel por ano (familias)</t>
-  </si>
-  <si>
-    <t>Mede o número de famílias beneficiárias de Auxílio Aluguel em cada ano usando como referência o mês de dezembro</t>
-  </si>
-  <si>
-    <t>O número de famílias beneficiárias de Auxílio Aluguél nos meses de dezembro permite uma comparação anual do fluxo de benefícios concedidos ao longo da série histórica.</t>
-  </si>
-  <si>
-    <t>Número de famílias beneficiárias de Auxílio Aluguel</t>
-  </si>
-  <si>
-    <t>ObservaSampa (HabitaSampa; Secretaria Municipal de Habitação (SEHAB)).</t>
-  </si>
-  <si>
-    <t>Auxílio Aluguel - Por Situação de Risco e Emergência</t>
-  </si>
-  <si>
-    <t>01.05.02 - Número de famílias em atendimento habitacional provisório (Auxílio Aluguel) por situação de risco e emergência (familias)</t>
-  </si>
-  <si>
-    <t>Mede a quantidade total de famílias em atendimento habitacional provisório pela SEHAB em um determinado período, que tenha como motivo da inclusão no benefício uma situação emergencial ou situação de risco, em um determinado período.</t>
-  </si>
-  <si>
-    <t>Número de famílias em atendimento habitacional provisório (Auxílio Aluguel) por situação de risco e emergência</t>
-  </si>
-  <si>
-    <t>ObservaSampa (Sistema Municipal de Informações Habitacionais (Habitasampa)/Secretaria Municipal de Habitação (SEHAB)/Departamento de Planejamento Habitacional (DEPLAN)).</t>
-  </si>
-  <si>
-    <t>Mapa de Parques Municipais e Estaduais</t>
-  </si>
-  <si>
-    <t>Área de Parque (%) por Subprefeitura (2024)</t>
-  </si>
-  <si>
-    <t>Mede a proporção da área ocupada por parques (municipais e estaduais) em relação à área total de cada subprefeitura no município de São Paulo.</t>
-  </si>
-  <si>
-    <t>Os polígonos de parques foram obtidos do GeoSampa (camada de Parques Existentes) e cruzados com os limites territoriais oficiais de cada subprefeitura. O indicador expressa o peso relativo das áreas de parques dentro de cada unidade administrativa, permitindo identificar diferenças na cobertura verde destinada a lazer e conservação ambiental.</t>
-  </si>
-  <si>
-    <t>Área de Parques na Subprefeitura (m²) ÷ Área Total da Subprefeitura (m²) × 100</t>
-  </si>
-  <si>
-    <t>GeoSampa</t>
-  </si>
-  <si>
-    <t>Parques, Área Permeável</t>
-  </si>
-  <si>
-    <t>Parques Novos e Requalificados e Áreas Permeáveis (2024) (%)</t>
-  </si>
-  <si>
-    <t>Mede a proporção de áreas permeáveis (incluindo parques, beiras de estrada e demais áreas não impermeabilizadas) em relação à área terrestre total do município, excluídas áreas marinhas sob jurisdição da cidade.</t>
-  </si>
-  <si>
-    <t>Área permeável total ÷ Área terrestre total da cidade × 100</t>
-  </si>
-  <si>
-    <t>Biosampa 2023 / Secretaria do Verde e do Meio Ambiente (SVMA-PMSP).</t>
-  </si>
-  <si>
-    <t>Valores Liquidados</t>
-  </si>
-  <si>
-    <t>Valores Liquidados (2024) - R$308.579.562,86 (Projeto 1702 + 1703) (R$)</t>
-  </si>
-  <si>
-    <t>Mede o valor liquidado do orçamento destinado por subprefeitura aos projetos e atividades 1702 (Construção e Implantação de Parques Urbanos e Lineares) e 1703 (Ampliação, Reforma e Requalificação de Parques Urbanos e Lineares).</t>
-  </si>
-  <si>
-    <t>Portal de Prestação de Contas Públicas / Secretaria Municipal da Fazenda (PMSP).</t>
-  </si>
-  <si>
-    <t>Déficit habitacional Municipal</t>
-  </si>
-  <si>
-    <t>11.01.01 - Déficit habitacional em relação ao total de domicílios (UN)</t>
-  </si>
-  <si>
-    <t>Não Disponível</t>
-  </si>
-  <si>
-    <t>São características principais do déficit habitacional, de acordo com o IPEA, a reposição de estoque e o incremento de estoque. A reposição de estoque contempla a necessidade de repor as habitações em função da sua precariedade e desgaste de uso. O incremento de estoque refere-se a demanda por novas moradias decorrente de: (a) coabitação forçada (aquela na qual a família convivente deseja constituir novo domicílio, mas não possui condições necessárias para tal); (b) famílias que residem em imóveis locados, com valores que comprometem mais de 30% da renda familiar; e (c) o adensamento excessivo em imóveis locados.</t>
-  </si>
-  <si>
-    <t>Número de domicílios com déficit ÷ Domicílios particulares permanentes × 100</t>
-  </si>
-  <si>
-    <t>ObservaSampa</t>
-  </si>
-  <si>
-    <t>Domicílios não ocupados</t>
-  </si>
-  <si>
-    <t>Domicílios não ocupados (UN)</t>
-  </si>
-  <si>
-    <t>Indica o número total de unidades habitacionais
-particulares existentes no território que, no momento da coleta censitária, não estavam sendo utilizadas como moradia principal.</t>
-  </si>
-  <si>
-    <t>São considerados domicílios não ocupados aqueles que, no momento da coleta do Censo Demográfico, não possuíam uso residencial ativo — incluindo tanto unidades vagas, sem moradores presentes, quanto domicílios ocupados sem entrevista, onde havia moradores mas a entrevista não foi realizada (por ausência ou recusa) — e domicílios de uso ocasional, utilizados apenas temporariamente para fins de descanso ou lazer.</t>
-  </si>
-  <si>
-    <t>Total de domicílios – Total de domicílios particulares permanentes ocupados</t>
-  </si>
-  <si>
-    <t>Censo Demográfico – Instituto Brasileiro de Geografia e Estatística (IBGE)/Elaboração própria</t>
-  </si>
-  <si>
-    <t>Domicílios não ocupados (%)</t>
-  </si>
-  <si>
-    <t>Indica o percentual em relação a subprefeitura de unidades habitacionais
-particulares existentes no território que, no momento da coleta censitária, não estavam sendo utilizadas como moradia principal.</t>
-  </si>
-  <si>
-    <t>Total de domicilios não ocupados ÷ Total de domicilios</t>
-  </si>
-  <si>
-    <t>Domicílios em Favelas</t>
-  </si>
-  <si>
-    <t>Número total de domicílios Favelas (UN)</t>
-  </si>
-  <si>
-    <t>Estimativa dos domicílios em favelas existentes em São Paulo</t>
-  </si>
-  <si>
-    <t>Número de domicilios em favela</t>
-  </si>
-  <si>
-    <t>ObservaSampa (Sistema Municipal de Informações Habitacionais (Habitasampa)/Secretaria Municipal de Habitação (SEHAB)</t>
-  </si>
-  <si>
-    <t>Unidades habitacionais entregues</t>
-  </si>
-  <si>
-    <t>Indicador 11.01.03 - Número de Unidades Habitacionais entregues (por meio de programas habitacionais e parcerias firmadas) (UN)</t>
-  </si>
-  <si>
-    <t>Apresenta a quantidade de Unidades Habitacionais entregues (por meio de programas habitacionais e parcerias firmadas).</t>
-  </si>
-  <si>
-    <t>Um elevado valor indica maior quantidade de
-Unidades Habitacionais entregues, o que represente um fortalecimento das políticas de moradia.</t>
-  </si>
-  <si>
-    <t>Unidades Habitacionais entregues (por meio de programas habitacionais e parcerias firmadas)</t>
-  </si>
-  <si>
-    <t>ObservaSampa (Sistema Municipal de
-Informações Habitacionais (Habitasampa)/Secretaria Municipal de Habitação (SEHAB)</t>
-  </si>
-  <si>
-    <t>Unidades habitacionais entregues e contratadas</t>
-  </si>
-  <si>
-    <t>Meta 12 do Programa de Metas 2021-2024 - Unidades habitacionais entregues e contratadas (UN)</t>
-  </si>
-  <si>
-    <t>O indicador considera as unidades entregues e contratadas por meio dos programas:
-Pode Entrar, Operações Urbanas Consorciadas, Parcerias Público-Privadas, Minha Casa Minha Vida, Casa Verde Amarela, Locação Social, Convênios e outros programas habitacionais.</t>
-  </si>
-  <si>
-    <t>Promover o acesso à moradia, à urbanização e à regularização fundiária para famílias de baixa renda.</t>
-  </si>
-  <si>
-    <t>Somatória do número de unidades habitacionais de interesse social, entregues e contratadas pelo poder público.</t>
-  </si>
-  <si>
-    <t>Programa de Metas – PMSP</t>
-  </si>
-  <si>
-    <t>Regularização fundiária urbana</t>
-  </si>
-  <si>
-    <t>Indicador 11.01.02 - Número de famílias beneficiadas por procedimentos de regularização fundiária em núcleos urbanos informais (familias)</t>
-  </si>
-  <si>
-    <t>Apresenta o número de famílias beneficiadas
-por procedimentos de regularização fundiária.</t>
-  </si>
-  <si>
-    <t>Um valor elevado desse número representa maior quantidades de famílias que usufruiram da regularização fundiária em núcleos urbanos informais.</t>
-  </si>
-  <si>
-    <t>Número de famílias beneficiadas por procedimentos de regularização fundiária em assentamentos precários</t>
-  </si>
-  <si>
-    <t>ObservaSampa/Secretaria Municipal de Habitação (SEHAB)</t>
-  </si>
-  <si>
-    <t>Obras em assentamentos precários</t>
-  </si>
-  <si>
-    <t>Indicador 11.01.06 - Número de famílias beneficiadas com obras de urbanização de assentamentos precários (familias)</t>
-  </si>
-  <si>
-    <t>Trata-se de famílias beneficiadas com as obras já iniciadas nesses territórios</t>
-  </si>
-  <si>
-    <t>Um valor elevado desse número representa maior quantidades de famílias que usufruiram das obras de urbanização de assentamentos precários.</t>
-  </si>
-  <si>
-    <t>Número de famílias beneficiadas com obras de urbanização de assentamentos precários em andamento</t>
-  </si>
-  <si>
-    <t>Orçado inicial</t>
-  </si>
-  <si>
-    <t>Valor orçado em reais</t>
-  </si>
-  <si>
-    <t>Valor orçamentário fixado pela Lei Orçamentária Anual. O valor aparece em relação a todo o orçamento muncipal, ou ao orçamento de cada função ou de cada projeto atividade.</t>
-  </si>
-  <si>
-    <t>É o valor aprovado na Lei Orçamentária Anual (LOA) no começo do ano. Representa a previsão oficial de quanto a prefeitura pretendia gastar e arrecadar em cada área antes de qualquer mudança. Serve como ponto de partida para acompanhar a execução orçamentária.</t>
-  </si>
-  <si>
-    <t>Valor orçado</t>
-  </si>
-  <si>
-    <t>Orçado atualizado</t>
-  </si>
-  <si>
-    <t>Valor atualizado em reais</t>
-  </si>
-  <si>
-    <t>Valor orçamentário vigente após as alterações ocorridas durante a execução orçamentária, considerando créditos adicionais (suplementações, anulações e remanejamentos)</t>
-  </si>
-  <si>
-    <t>É o orçamento inicial ajustado pelas modificações legais e infralegais ocorridas ao longo do exercício, refletindo a dotação disponível para execução.</t>
-  </si>
-  <si>
-    <t>Valor orçado + suplementação líquida</t>
-  </si>
-  <si>
-    <t>Variação em relação ao orçamento inicial (R$)</t>
-  </si>
-  <si>
-    <t>Suplementação líquida em reais</t>
-  </si>
-  <si>
-    <t>Indica o valor nominal da suplementação líquida. O valor aparece em relação a todo o orçamento muncipal, ou ao orçamento de cada função ou de cada projeto atividade.</t>
-  </si>
-  <si>
-    <t>Representa o aumento de recursos por crédito adicional, para reforçar as dotações que já constam na lei orçamentária, descontando-se as deduções.</t>
-  </si>
-  <si>
-    <t>Suplementação líquida</t>
-  </si>
-  <si>
-    <t>Variação em relação ao orçamento inicial (%)</t>
-  </si>
-  <si>
-    <t>Suplementação líquida em relação ao orçamento inicial</t>
-  </si>
-  <si>
-    <t>Indica o valor percentual da suplementação líquida em relação ao valor orçado inicial. O valor aparece em relação a todo o orçamento muncipal, ou ao orçamento de cada função ou de cada projeto atividade.</t>
-  </si>
-  <si>
-    <t>Representa o aumento de recursos por crédito adicional, para reforçar as dotações que já constam na lei orçamentária, descontando-se as deduções. O valor é apresentado em formato percentual, relativo ao valor orçado inicial do escopo analisado.</t>
-  </si>
-  <si>
-    <t>Suplementação líquida ÷ Orçamento inicial × 100</t>
-  </si>
-  <si>
-    <t>Variação da participação relativa no orçamento (%)</t>
-  </si>
-  <si>
-    <t>Variação da participação relativa no orçamento</t>
-  </si>
-  <si>
-    <t>Valor percentual da variação entre a participação relativa de cada função de governo no orçamento municipal.</t>
-  </si>
-  <si>
-    <t>Representa a variação da importância relativa de cada função de governo dentro do orçamento municipal</t>
-  </si>
-  <si>
-    <t>[(Orçamento atualizado da função ÷ Orçamento atualizado do Município) - (Orçamento inicial da função ÷ Orçamento inicial do Município)] ÷ (Orçamento inicial da função ÷ Orçamento inicial do Município)</t>
-  </si>
-  <si>
-    <t>Prestação de Contas Públicas - Orçamento, PMSP; Elaboração Própria</t>
-  </si>
-  <si>
-    <t>Liquidado</t>
-  </si>
-  <si>
-    <t>Valor liquidado em reais</t>
-  </si>
-  <si>
-    <t>Somatório de todas as Notas de Liquidação e Pagamento emitidas. O valor aparece em relação a todo o orçamento muncipal, ou ao orçamento de cada função ou de cada projeto atividade.</t>
-  </si>
-  <si>
-    <t>Valor liquidado</t>
+  </si>
+  <si>
+    <t>Despesas "per capita" em Atenção Básica e Vigilãncia Sanitária= valor em reais do orçamento municipal executado em atenção primária (UBS, AMA) e vigilância sanitária ÷ população residente no município (em Reais÷hab)</t>
+  </si>
+  <si>
+    <t>Despesas "per capita" em Atenção Especializada e Suporte Profilático e Terapêutico = valor em reais do orçamento municipal executado em atenção hospitalar, pré-hospitalar (SAMU) e emergencial (UPAs)  ÷ população residente no município (em Reais÷hab)</t>
+  </si>
+  <si>
+    <t>Densidade Demográfica= população residente no município ÷ área do município em km2</t>
+  </si>
+  <si>
+    <t>Taxa de Mortalidade por Causas Evitáveis= nº de óbitos por causas evitáveis ÷ população do município × 100.000</t>
+  </si>
+  <si>
+    <t>Taxa de Mortalidade por Causas Tratáveis= nº de óbitos por causas tratáveis ÷ população do município × 100.000</t>
+  </si>
+  <si>
+    <t>Taxa de Mortalidade por Causas Evitáveis÷ Tratáveis= nº de óbitos por causas evitáveis + tratáveis ÷ população do município × 100.000</t>
+  </si>
+  <si>
+    <t>Média Anual de Leitos de Internação por Habitante= média anual de leitos de internação hospitalar ÷ população residente no município × 100.000</t>
+  </si>
+  <si>
+    <t>Média Anual de Leitos Complementares por Habitante = média anual de leitos complementares no SUS ÷ população residente no município × 100.000</t>
+  </si>
+  <si>
+    <t>Média Anual de Leitos de UTI por Habitante = média anual de leitos de UTI no SUS ÷ população residente no município × 100.000</t>
+  </si>
+  <si>
+    <t>Percentual de Idosos =  população com 60 anos e mais ÷ população total residente no município × 100</t>
+  </si>
+  <si>
+    <t>PIB "per capita"= produto interno bruto do município ÷ população residente no município × 100</t>
+  </si>
+  <si>
+    <t>Percentual de Usuários de Planos de Privados de Saúde= número de usuários de planos ÷ população residente no município × 100</t>
   </si>
 </sst>
 </file>
@@ -1003,11 +1048,12 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1106,7 +1152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1178,130 +1224,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="49">
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="12"/>
-        <name val="Arial"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1329,7 +1262,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1344,7 +1277,126 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1824,48 +1876,48 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{54F881FD-9F9A-4FAB-8992-625B38656F73}" name="Tabela5" displayName="Tabela5" ref="A1:G5" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="A1:G5" xr:uid="{31912C27-6982-4EC1-913B-26A0A82C5565}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{54F881FD-9F9A-4FAB-8992-625B38656F73}" name="Tabela5" displayName="Tabela5" ref="A1:G15" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="A1:G15" xr:uid="{31912C27-6982-4EC1-913B-26A0A82C5565}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DA9D5663-9415-47B7-9F4B-71B8FD57C054}" name="Indicador resumido" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{DDFEC43D-78E3-4C46-866F-CDC2042BF6D8}" name="Indicador completo" dataDxfId="23"/>
     <tableColumn id="3" xr3:uid="{4D0F4D41-4090-4AD0-B9CC-D25A8FE5043D}" name="Descrição" dataDxfId="22"/>
     <tableColumn id="4" xr3:uid="{0607F75E-860D-4465-9653-150D5F60DCCD}" name="Conceito" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{3BFA8B5B-609F-4FDF-831B-73333B92D0EC}" name="Fórmula de cálculo" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{4F5EB453-26BC-4372-B12E-5224C85FCE0A}" name="Fonte" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{22DDF6F2-E3E7-4C0C-B34E-F8B6D88F9F24}" name="Ano de referência" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{3BFA8B5B-609F-4FDF-831B-73333B92D0EC}" name="Fórmula de cálculo" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4F5EB453-26BC-4372-B12E-5224C85FCE0A}" name="Fonte" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{22DDF6F2-E3E7-4C0C-B34E-F8B6D88F9F24}" name="Ano de referência" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71EB0227-08CA-444F-817B-FB88087A057B}" name="Tabela1" displayName="Tabela1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71EB0227-08CA-444F-817B-FB88087A057B}" name="Tabela1" displayName="Tabela1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:G22" xr:uid="{8B9764C9-251E-4087-8400-38B5AB15EA5C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A2328E45-F2BF-490D-8793-CC87E9496015}" name="Indicador resumido" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{7E466F10-5210-4E12-94C0-A7F98F2FA1B6}" name="Indicador completo" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{9B03C3B3-577B-41E1-BFC6-C4D0DF6E6B9D}" name="Descrição" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{B7BA94A7-3B23-45B4-9CDB-E6C5199ABF4A}" name="Conceito" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{7F89F049-ABC7-40D9-B067-2A51764C50C7}" name="Fórmula de cálculo" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{01005479-EA15-443D-81A0-B205BE7422BD}" name="Fonte" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{0E922A3C-E19E-4DDC-AC98-57B1ED10E71B}" name="Ano de referência" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{A2328E45-F2BF-490D-8793-CC87E9496015}" name="Indicador resumido" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{7E466F10-5210-4E12-94C0-A7F98F2FA1B6}" name="Indicador completo" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{9B03C3B3-577B-41E1-BFC6-C4D0DF6E6B9D}" name="Descrição" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{B7BA94A7-3B23-45B4-9CDB-E6C5199ABF4A}" name="Conceito" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{7F89F049-ABC7-40D9-B067-2A51764C50C7}" name="Fórmula de cálculo" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{01005479-EA15-443D-81A0-B205BE7422BD}" name="Fonte" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{0E922A3C-E19E-4DDC-AC98-57B1ED10E71B}" name="Ano de referência" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1261AC3D-D1F8-457C-B001-04401448163B}" name="Tabela2" displayName="Tabela2" ref="A1:G7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1261AC3D-D1F8-457C-B001-04401448163B}" name="Tabela2" displayName="Tabela2" ref="A1:G7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:G7" xr:uid="{20592E48-E74A-429A-8684-955A95EF456D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AE4FBE35-E209-448E-A89D-EFBCAF45A5A8}" name="Indicador resumido" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{06A67404-41B3-4F09-A2DE-0F395BB44518}" name="Indicador completo" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B89867C4-CA5A-44E5-AD82-0F5EFABC9C29}" name="Descrição" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{C387C4D6-C20A-48E4-8E84-7E3EA337FC99}" name="Conceito" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{D743CEFC-34AA-4D03-AF3F-ED1D00E6D8B1}" name="Fórmula de cálculo" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{1DBABDF0-06AE-43D5-BEA7-7FC03AC462C9}" name="Fonte" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{E5385D92-36B7-4A87-A9DA-1120739752A1}" name="Ano de referência" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{AE4FBE35-E209-448E-A89D-EFBCAF45A5A8}" name="Indicador resumido" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{06A67404-41B3-4F09-A2DE-0F395BB44518}" name="Indicador completo" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{B89867C4-CA5A-44E5-AD82-0F5EFABC9C29}" name="Descrição" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{C387C4D6-C20A-48E4-8E84-7E3EA337FC99}" name="Conceito" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{D743CEFC-34AA-4D03-AF3F-ED1D00E6D8B1}" name="Fórmula de cálculo" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{1DBABDF0-06AE-43D5-BEA7-7FC03AC462C9}" name="Fonte" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{E5385D92-36B7-4A87-A9DA-1120739752A1}" name="Ano de referência" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2193,16 +2245,16 @@
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="25" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="47.625" customWidth="1"/>
+    <col min="4" max="4" width="50.75" customWidth="1"/>
+    <col min="5" max="5" width="38.625" customWidth="1"/>
+    <col min="6" max="6" width="25.125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2435,17 +2487,17 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="9" customWidth="1"/>
     <col min="2" max="2" width="28" style="21" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" style="21" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" style="21" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="47.625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="50.75" style="21" customWidth="1"/>
+    <col min="5" max="5" width="38.625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="25.125" style="9" customWidth="1"/>
     <col min="7" max="7" width="17" style="9" customWidth="1"/>
     <col min="8" max="16384" width="9" style="9"/>
   </cols>
@@ -2786,20 +2838,20 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="47.625" customWidth="1"/>
+    <col min="4" max="4" width="50.75" customWidth="1"/>
+    <col min="5" max="5" width="38.625" customWidth="1"/>
+    <col min="6" max="6" width="25.125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2826,87 +2878,325 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="75">
-      <c r="A2" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" s="22">
+    <row r="2" spans="1:7" ht="99.75">
+      <c r="A2" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="G2" s="28">
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="60.75">
-      <c r="A3" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" s="22">
+    <row r="3" spans="1:7" ht="99.75">
+      <c r="A3" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" s="28">
         <v>2024</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="74.25">
-      <c r="A4" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" s="22">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="75.75">
-      <c r="A5" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="22">
+    <row r="4" spans="1:7" ht="85.5">
+      <c r="A4" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4" s="28">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="99.75">
+      <c r="A5" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="G5" s="28">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="99.75">
+      <c r="A6" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="G6" s="20">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="71.25">
+      <c r="A7" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="G7" s="20">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="75">
+      <c r="A8" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="G8" s="20">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="105">
+      <c r="A9" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="G9" s="20">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45">
+      <c r="A10" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="G10" s="20">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45">
+      <c r="A11" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="G11" s="20">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45">
+      <c r="A12" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="G12" s="20">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="75">
+      <c r="A13" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="G13" s="20">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45">
+      <c r="A14" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="G14" s="20">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="105">
+      <c r="A15" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>295</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="G15" s="20">
         <v>2024</v>
       </c>
     </row>
@@ -2926,16 +3216,18 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="9" customWidth="1"/>
     <col min="2" max="2" width="28" style="9" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="47.625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="50.75" style="9" customWidth="1"/>
+    <col min="5" max="5" width="38.625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="25.125" style="9" customWidth="1"/>
     <col min="7" max="7" width="17" style="9" customWidth="1"/>
     <col min="8" max="16384" width="9" style="9"/>
   </cols>
@@ -2965,183 +3257,183 @@
     </row>
     <row r="2" spans="1:7" ht="90">
       <c r="A2" s="17" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="75">
       <c r="A3" s="16" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="90">
       <c r="A4" s="17" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75">
       <c r="A5" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>124</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75">
       <c r="A6" s="17" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="90">
       <c r="A7" s="16" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="270">
       <c r="A8" s="17" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="60">
       <c r="A9" s="16" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="G9" s="13">
         <v>2024</v>
@@ -3149,22 +3441,22 @@
     </row>
     <row r="10" spans="1:7" ht="60">
       <c r="A10" s="17" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="G10" s="11">
         <v>2024</v>
@@ -3172,22 +3464,22 @@
     </row>
     <row r="11" spans="1:7" ht="120">
       <c r="A11" s="16" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="D11" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>135</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>154</v>
       </c>
       <c r="G11" s="13">
         <v>2024</v>
@@ -3195,22 +3487,22 @@
     </row>
     <row r="12" spans="1:7" ht="105">
       <c r="A12" s="17" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G12" s="11">
         <v>2024</v>
@@ -3218,22 +3510,22 @@
     </row>
     <row r="13" spans="1:7" ht="75">
       <c r="A13" s="16" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="G13" s="13">
         <v>2024</v>
@@ -3241,22 +3533,22 @@
     </row>
     <row r="14" spans="1:7" ht="75">
       <c r="A14" s="17" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="G14" s="11">
         <v>2024</v>
@@ -3264,22 +3556,22 @@
     </row>
     <row r="15" spans="1:7" ht="195">
       <c r="A15" s="16" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="G15" s="13">
         <v>2022</v>
@@ -3287,68 +3579,68 @@
     </row>
     <row r="16" spans="1:7" ht="135">
       <c r="A16" s="17" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="135">
       <c r="A17" s="16" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="90">
       <c r="A18" s="17" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="G18" s="11">
         <v>2024</v>
@@ -3356,43 +3648,43 @@
     </row>
     <row r="19" spans="1:7" ht="90">
       <c r="A19" s="16" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:7" ht="90">
       <c r="A20" s="17" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="G20" s="11">
         <v>2024</v>
@@ -3400,22 +3692,22 @@
     </row>
     <row r="21" spans="1:7" ht="90">
       <c r="A21" s="16" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="G21" s="13">
         <v>2024</v>
@@ -3423,22 +3715,22 @@
     </row>
     <row r="22" spans="1:7" ht="75">
       <c r="A22" s="17" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="G22" s="11">
         <v>2024</v>
@@ -3464,12 +3756,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="47.625" customWidth="1"/>
+    <col min="4" max="4" width="50.75" customWidth="1"/>
+    <col min="5" max="5" width="38.625" customWidth="1"/>
+    <col min="6" max="6" width="25.125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3498,22 +3790,22 @@
     </row>
     <row r="2" spans="1:7" ht="90">
       <c r="A2" s="1" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G2" s="4">
         <v>2024</v>
@@ -3521,22 +3813,22 @@
     </row>
     <row r="3" spans="1:7" ht="60">
       <c r="A3" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G3" s="4">
         <v>2024</v>
@@ -3544,22 +3836,22 @@
     </row>
     <row r="4" spans="1:7" ht="60">
       <c r="A4" s="1" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G4" s="4">
         <v>2024</v>
@@ -3567,22 +3859,22 @@
     </row>
     <row r="5" spans="1:7" ht="75">
       <c r="A5" s="1" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G5" s="4">
         <v>2024</v>
@@ -3590,22 +3882,22 @@
     </row>
     <row r="6" spans="1:7" ht="90">
       <c r="A6" s="1" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="G6" s="4">
         <v>2024</v>
@@ -3613,22 +3905,22 @@
     </row>
     <row r="7" spans="1:7" ht="75">
       <c r="A7" s="1" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G7" s="4">
         <v>2024</v>
@@ -3644,23 +3936,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bd2b4508-43bb-43a9-949a-527d9edee5a0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006395861A52F15448BD3944CBD4C58617" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee4bdd7030f0ea7859f0af66fe99e547">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bd2b4508-43bb-43a9-949a-527d9edee5a0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="719c67f33cf9376c21946e0c443abf4c" ns3:_="">
     <xsd:import namespace="bd2b4508-43bb-43a9-949a-527d9edee5a0"/>
@@ -3848,14 +4123,55 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bd2b4508-43bb-43a9-949a-527d9edee5a0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1ADD084-BC56-46F9-993B-1BFE8BDA123B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D656A5-8B52-4FDF-93EC-791B5E719C59}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bd2b4508-43bb-43a9-949a-527d9edee5a0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0753EEC0-270F-4C9C-9E87-6EB2D8E16582}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0753EEC0-270F-4C9C-9E87-6EB2D8E16582}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D656A5-8B52-4FDF-93EC-791B5E719C59}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1ADD084-BC56-46F9-993B-1BFE8BDA123B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bd2b4508-43bb-43a9-949a-527d9edee5a0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
234 saude adicionar dados de obitos ao site (#238)
* Arquivo de mortalidade ajustado para faixa etaria de 0 a 69 anos

* Arquivos da saude atualizados

* Links dos arquivos atualizados

* Metadados atualizado
</commit_message>
<xml_diff>
--- a/public/infos/metadados-datasp.xlsx
+++ b/public/infos/metadados-datasp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\855395\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b_bal\git\painel-frontend\public\infos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183DC683-7829-4195-B067-F6EE5E3E96AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8F8F1B-AAC1-4AA0-9437-2D74A56C9B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10125" activeTab="2" xr2:uid="{5C405DEB-DBE8-4978-A59C-3D6D75628EC4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{5C405DEB-DBE8-4978-A59C-3D6D75628EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="GT Educação" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="262">
   <si>
     <t>Indicador resumido</t>
   </si>
@@ -744,24 +744,15 @@
     <t>Taxa de Mortalidade por Causas Evitáveis / 100 mil hab.</t>
   </si>
   <si>
-    <t>Indica a quantidade relativa de mortes que ocorrem por causas para as quais existe prevenção conhecida e eficaz</t>
-  </si>
-  <si>
     <t>Representa a quantidade de mortes que poderiam ser evitadas se o método de prevenção (p. ex. vacinas) ou  ações educativas e terapêuticas contra fatores de risco (p. ex. obesidade, hipertensão arterial, diabetes mellitus, etc...) estivessem disponíveis na fase evitável da doença. Este indicador tem relação direta com o investimento de recursos públicos na Atenção Primária em Saúde.</t>
   </si>
   <si>
-    <t>SIM - Sistema de Informação sobre Mortalidade; IBGE -  Instituto Bbrasileiro de Geografia e Estatística</t>
-  </si>
-  <si>
     <t>Mortalidade por Causas Tratáveis</t>
   </si>
   <si>
     <t>Taxa de Mortalidade por Causas Tratáveis / 100 mil hab.</t>
   </si>
   <si>
-    <t>Indica a quantidade relativa de mortes que ocorrem por causas para as quais existem tratamentos conhecidos e eficazes.</t>
-  </si>
-  <si>
     <t>Representa a quantidade de mortes que poderiam não acontecer se os métodos de diagnóstico precoce e tratamento oportuno (p. ex. Câncer de Colo Uterino, Diabetes Mellitus, etc...)  fossem realizados no momento oportuno do desenvolvimento da doença. Este indicador tem relação direta com o investimento de recursos públicos na Atenção Especializada e Hospittalar.</t>
   </si>
   <si>
@@ -771,9 +762,6 @@
     <t>Taxa de Mortalidade por Causas Evitáveis/Tratáveis / 100 mil hab.</t>
   </si>
   <si>
-    <t>Indica a somatória das quantidades relativas de mortes que ocorrem por causas para as quais existe prevenção conhecida e eficaz e por cacusas para as quais existem tratamentos conhecidos e eficazes.</t>
-  </si>
-  <si>
     <t>Este indicador elimina a quantidade relativa de mortes por causas que independem da administração pública (p. ex. doenças genéticas, congênitas, hereditárias, etc...) e evidencia a quantidade relativa de mortes que em tese poderia ser impactada por ações do investimento público em Saúde.</t>
   </si>
   <si>
@@ -783,24 +771,15 @@
     <t>Despesas "per capita" em Atenção Primária e Vigilância Sanitária / hab.</t>
   </si>
   <si>
-    <t xml:space="preserve">Indica o montante do investimento público em ações de promoção da saúde e prevenção de doenças. </t>
-  </si>
-  <si>
     <t>Representa o volume de investimento de recursos públicos em saúde ANTES do surgimento das doenças.</t>
   </si>
   <si>
-    <t>IBGE -  Instituto Bbrasileiro de Geografia e Estatística; SIOPS - Sistema de Informações sobre Orçamentos Públicos em Saúde; FNS - Fundo Nacional de Saúde</t>
-  </si>
-  <si>
     <t>Despesas "per capita" em Atenção Especializada</t>
   </si>
   <si>
     <t>Despesas "per capita" em Atenção Especializada e Suporte Profilático Terapêutico / hab</t>
   </si>
   <si>
-    <t>Indica o montante do investimento de recursos públicos em ações curativas e de reabilitação</t>
-  </si>
-  <si>
     <t>Representa o volume de investimento de recursos públicos em tratamento, DEPOIS que a doença já se instalou, e necessita de atendimento de urgência (UPAs) e de tratamento hospitalar especializado.</t>
   </si>
   <si>
@@ -813,166 +792,21 @@
     <t>Representa o volume de investimento de recursos públicos em tratamento, DEPOIS que a doença já se instalou, e necessita de tratamento hospitalar especializado.</t>
   </si>
   <si>
-    <t>IBGE -  Instituto Bbrasileiro de Geografia e Estatística; CNES - Cadastro Nacional de Estabelecimentos de Saúde</t>
-  </si>
-  <si>
     <t>Leitos Complementares</t>
   </si>
   <si>
     <t>Leitos Complementares / 100 mil hab.</t>
   </si>
   <si>
-    <t>Indica o montante do investimento de recursos públicos em atendimento a situações de urgência e emergências, como leitos de Salas de Emergência  e de Salas de Observação em Pronto Socorros e UPAs.</t>
-  </si>
-  <si>
     <t>Representa o volume de investimento de recursos públicos em Salas de Emergência  e Salas de Observação em Pronto Socorros e UPAs,  onde o risco de morte é importante ou iminente.</t>
   </si>
   <si>
-    <t>Leitos de UTI</t>
-  </si>
-  <si>
-    <t>Equipamentos respiradores e ventiladores / 100 mil hab.</t>
-  </si>
-  <si>
-    <t>Indica o montante do investimento de recursos públicos em atendimento a situações de alta gravidade, com allrisco de morte.</t>
-  </si>
-  <si>
-    <t>Representa o volume de investimento de recursos públicos em equipamentos de de atendimento a situações de alto risco de morte iminente. Em muitas situações este equipamento é usado para tratar  eventos de alta gravidade que poderiam ter sido evitados com programas eficazes de promoção da saúde e prevenção de doenças.</t>
-  </si>
-  <si>
-    <t>População</t>
-  </si>
-  <si>
-    <t>População (x 1 mil hab.)</t>
-  </si>
-  <si>
-    <t>Indica a qauntidade de pessoas que habitam o território do município</t>
-  </si>
-  <si>
-    <t>Representa um indicadoo importante para dimensionar corretamente a importância e o impacto dos demais indicadores deste conjunto.</t>
-  </si>
-  <si>
-    <t>Número absoluto de habitantes (em milhares)</t>
-  </si>
-  <si>
-    <t>IBGE -  Instituto Bbrasileiro de Geografia e Estatística</t>
-  </si>
-  <si>
-    <t>Área</t>
-  </si>
-  <si>
-    <t>Indica a dimensão do território considerado na anãlise dos investimentos de recursos públicos</t>
-  </si>
-  <si>
-    <t>Número absoluto de km2 da área municipal</t>
-  </si>
-  <si>
-    <t>Densidade Demográfica</t>
-  </si>
-  <si>
-    <t>Indica a quantidade de pessoas por unidade de território</t>
-  </si>
-  <si>
-    <t>Idosos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porcentagem de Idosos (%) </t>
-  </si>
-  <si>
-    <t>Indica a proporção de idosos na população geral do território</t>
-  </si>
-  <si>
-    <t>Representa um recorte importante do panorama da necessidade de açoes de saúde na população. A porcentagem de idosos indica a demanda de ações de saúde preventivas e curativas a longo prazo, impactando a destinação  de recursos públicos.</t>
-  </si>
-  <si>
-    <t>PIB "per capita"</t>
-  </si>
-  <si>
-    <t>Produto Interno Bruto "per capita"</t>
-  </si>
-  <si>
-    <t>Indica a quantidade de recursos públicos que estará disponível para investimento nas nececssidades sociais.</t>
-  </si>
-  <si>
-    <t>Representa o limite dos recursos disponíveis para investimento nas necessidades sociais</t>
-  </si>
-  <si>
-    <t>Usuários de Planos de Saúde</t>
-  </si>
-  <si>
-    <t>Porcentagem de Usuários de Planos de Saúde Privados (%)</t>
-  </si>
-  <si>
-    <t>Indica  a quantidade relativa de habitantes que são usuário de serviçoos de saúde privados, independentes dos recursos públicos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Representa a quantidade relativa da população que utiliza recursos privados para a assistência à saúde. É importante notar que essa parcela da população não consome recursos do SUS na Assistência Especializada Ambulatorial e Hospitalar, mas vai recorrer ao SUS nas situaçãoes de maior custo, como tratamento de câncer e transplantes de órgãos. </t>
-  </si>
-  <si>
-    <t>ANS - Agência Nacional de Saúde Suplementar</t>
-  </si>
-  <si>
-    <r>
-      <t>Área (km</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Densidade Demográfica (hab./km</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>Despesas "per capita" em Atenção Básica e Vigilãncia Sanitária= valor em reais do orçamento municipal executado em atenção primária (UBS, AMA) e vigilância sanitária ÷ população residente no município (em Reais÷hab)</t>
   </si>
   <si>
     <t>Despesas "per capita" em Atenção Especializada e Suporte Profilático e Terapêutico = valor em reais do orçamento municipal executado em atenção hospitalar, pré-hospitalar (SAMU) e emergencial (UPAs)  ÷ população residente no município (em Reais÷hab)</t>
   </si>
   <si>
-    <t>Densidade Demográfica= população residente no município ÷ área do município em km2</t>
-  </si>
-  <si>
     <t>Taxa de Mortalidade por Causas Evitáveis= nº de óbitos por causas evitáveis ÷ população do município × 100.000</t>
   </si>
   <si>
@@ -988,23 +822,41 @@
     <t>Média Anual de Leitos Complementares por Habitante = média anual de leitos complementares no SUS ÷ população residente no município × 100.000</t>
   </si>
   <si>
-    <t>Média Anual de Leitos de UTI por Habitante = média anual de leitos de UTI no SUS ÷ população residente no município × 100.000</t>
-  </si>
-  <si>
-    <t>Percentual de Idosos =  população com 60 anos e mais ÷ população total residente no município × 100</t>
-  </si>
-  <si>
-    <t>PIB "per capita"= produto interno bruto do município ÷ população residente no município × 100</t>
-  </si>
-  <si>
-    <t>Percentual de Usuários de Planos de Privados de Saúde= número de usuários de planos ÷ população residente no município × 100</t>
+    <t>Indica o montante do investimento público em ações de promoção da saúde e prevenção de doenças. A população do município utilizada no cálculo da taxa por habitante considera apenas o limite de idade de 0 a 74 anos, conforme é utilizado na OCDE e na UE.</t>
+  </si>
+  <si>
+    <t>Indica a somatória das quantidades relativas de mortes que ocorrem por causas para as quais existe prevenção conhecida e eficaz e por cacusas para as quais existem tratamentos conhecidos e eficazes. Tanto os óbitos, quanto a população do município utilizada no cálculo da taxa, consideram apenas o limite de idade de 0 a 74 anos, conforme é utilizado na OCDE e na UE.</t>
+  </si>
+  <si>
+    <t>Indica a quantidade relativa de mortes que ocorrem por causas para as quais existem tratamentos conhecidos e eficazes. Tanto os óbitos, quanto a população do município utilizada no cálculo da taxa, consideram apenas o limite de idade de 0 a 74 anos, conforme é utilizado na OCDE e na UE.</t>
+  </si>
+  <si>
+    <t>Indica a quantidade relativa de mortes que ocorrem por causas para as quais existe prevenção conhecida e eficaz. Tanto os óbitos, quanto a população do município utilizada no cálculo da taxa, consideram apenas o limite de idade de 0 a 74 anos, conforme é utilizado na OCDE e na UE.</t>
+  </si>
+  <si>
+    <t>Indica o montante do investimento de recursos públicos em ações curativas e de reabilitação.  A população do município utilizada no cálculo da taxa por habitante considera apenas o limite de idade de 0 a 74 anos, conforme é utilizado na OCDE e na UE.</t>
+  </si>
+  <si>
+    <t>Indica o montante do investimento de recursos públicos em ações curativas e de reabilitação.  A população do município utilizada no cálculo da taxa por 100 mil habitantes considera apenas o limite de idade de 0 a 74 anos, conforme é utilizado na OCDE e na UE.</t>
+  </si>
+  <si>
+    <t>Indica o montante do investimento de recursos públicos em atendimento a situações de urgência e emergências, como leitos de Salas de Emergência  e de Salas de Observação em Pronto Socorros e UPAs.  A população do município utilizada no cálculo da taxa por 100 mil habitantes considera apenas o limite de idade de 0 a 74 anos, conforme é utilizado na OCDE e na UE.</t>
+  </si>
+  <si>
+    <t>SIM - Sistema de Informação sobre Mortalidade; Fundação SEADE</t>
+  </si>
+  <si>
+    <t>Fundação SEADE; SIOPS - Sistema de Informações sobre Orçamentos Públicos em Saúde; FNS - Fundo Nacional de Saúde</t>
+  </si>
+  <si>
+    <t>Fundação SEADE; CNES - Cadastro Nacional de Estabelecimentos de Saúde</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1017,16 +869,19 @@
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1046,14 +901,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1152,7 +999,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1225,10 +1072,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1248,6 +1092,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1262,7 +1107,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1277,126 +1122,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="12"/>
-        <name val="Arial"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1411,7 +1137,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1426,7 +1152,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1441,7 +1167,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1456,7 +1182,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1471,7 +1197,126 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1876,48 +1721,48 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{54F881FD-9F9A-4FAB-8992-625B38656F73}" name="Tabela5" displayName="Tabela5" ref="A1:G15" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="A1:G15" xr:uid="{31912C27-6982-4EC1-913B-26A0A82C5565}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{54F881FD-9F9A-4FAB-8992-625B38656F73}" name="Tabela5" displayName="Tabela5" ref="A1:G8" totalsRowShown="0" headerRowDxfId="26" dataDxfId="3">
+  <autoFilter ref="A1:G8" xr:uid="{31912C27-6982-4EC1-913B-26A0A82C5565}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DA9D5663-9415-47B7-9F4B-71B8FD57C054}" name="Indicador resumido" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{DDFEC43D-78E3-4C46-866F-CDC2042BF6D8}" name="Indicador completo" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{4D0F4D41-4090-4AD0-B9CC-D25A8FE5043D}" name="Descrição" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{0607F75E-860D-4465-9653-150D5F60DCCD}" name="Conceito" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{DA9D5663-9415-47B7-9F4B-71B8FD57C054}" name="Indicador resumido" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{DDFEC43D-78E3-4C46-866F-CDC2042BF6D8}" name="Indicador completo" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{4D0F4D41-4090-4AD0-B9CC-D25A8FE5043D}" name="Descrição" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{0607F75E-860D-4465-9653-150D5F60DCCD}" name="Conceito" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{3BFA8B5B-609F-4FDF-831B-73333B92D0EC}" name="Fórmula de cálculo" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4F5EB453-26BC-4372-B12E-5224C85FCE0A}" name="Fonte" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{22DDF6F2-E3E7-4C0C-B34E-F8B6D88F9F24}" name="Ano de referência" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{4F5EB453-26BC-4372-B12E-5224C85FCE0A}" name="Fonte" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{22DDF6F2-E3E7-4C0C-B34E-F8B6D88F9F24}" name="Ano de referência" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71EB0227-08CA-444F-817B-FB88087A057B}" name="Tabela1" displayName="Tabela1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71EB0227-08CA-444F-817B-FB88087A057B}" name="Tabela1" displayName="Tabela1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:G22" xr:uid="{8B9764C9-251E-4087-8400-38B5AB15EA5C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A2328E45-F2BF-490D-8793-CC87E9496015}" name="Indicador resumido" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{7E466F10-5210-4E12-94C0-A7F98F2FA1B6}" name="Indicador completo" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{9B03C3B3-577B-41E1-BFC6-C4D0DF6E6B9D}" name="Descrição" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{B7BA94A7-3B23-45B4-9CDB-E6C5199ABF4A}" name="Conceito" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{7F89F049-ABC7-40D9-B067-2A51764C50C7}" name="Fórmula de cálculo" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{01005479-EA15-443D-81A0-B205BE7422BD}" name="Fonte" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{0E922A3C-E19E-4DDC-AC98-57B1ED10E71B}" name="Ano de referência" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{A2328E45-F2BF-490D-8793-CC87E9496015}" name="Indicador resumido" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{7E466F10-5210-4E12-94C0-A7F98F2FA1B6}" name="Indicador completo" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{9B03C3B3-577B-41E1-BFC6-C4D0DF6E6B9D}" name="Descrição" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{B7BA94A7-3B23-45B4-9CDB-E6C5199ABF4A}" name="Conceito" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{7F89F049-ABC7-40D9-B067-2A51764C50C7}" name="Fórmula de cálculo" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{01005479-EA15-443D-81A0-B205BE7422BD}" name="Fonte" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{0E922A3C-E19E-4DDC-AC98-57B1ED10E71B}" name="Ano de referência" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1261AC3D-D1F8-457C-B001-04401448163B}" name="Tabela2" displayName="Tabela2" ref="A1:G7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1261AC3D-D1F8-457C-B001-04401448163B}" name="Tabela2" displayName="Tabela2" ref="A1:G7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:G7" xr:uid="{20592E48-E74A-429A-8684-955A95EF456D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AE4FBE35-E209-448E-A89D-EFBCAF45A5A8}" name="Indicador resumido" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{06A67404-41B3-4F09-A2DE-0F395BB44518}" name="Indicador completo" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{B89867C4-CA5A-44E5-AD82-0F5EFABC9C29}" name="Descrição" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{C387C4D6-C20A-48E4-8E84-7E3EA337FC99}" name="Conceito" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{D743CEFC-34AA-4D03-AF3F-ED1D00E6D8B1}" name="Fórmula de cálculo" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{1DBABDF0-06AE-43D5-BEA7-7FC03AC462C9}" name="Fonte" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{E5385D92-36B7-4A87-A9DA-1120739752A1}" name="Ano de referência" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{AE4FBE35-E209-448E-A89D-EFBCAF45A5A8}" name="Indicador resumido" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{06A67404-41B3-4F09-A2DE-0F395BB44518}" name="Indicador completo" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{B89867C4-CA5A-44E5-AD82-0F5EFABC9C29}" name="Descrição" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{C387C4D6-C20A-48E4-8E84-7E3EA337FC99}" name="Conceito" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{D743CEFC-34AA-4D03-AF3F-ED1D00E6D8B1}" name="Fórmula de cálculo" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{1DBABDF0-06AE-43D5-BEA7-7FC03AC462C9}" name="Fonte" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{E5385D92-36B7-4A87-A9DA-1120739752A1}" name="Ano de referência" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2245,20 +2090,22 @@
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="25.59765625" style="25" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="47.625" customWidth="1"/>
-    <col min="4" max="4" width="50.75" customWidth="1"/>
-    <col min="5" max="5" width="38.625" customWidth="1"/>
-    <col min="6" max="6" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="47.59765625" customWidth="1"/>
+    <col min="4" max="4" width="50.73046875" customWidth="1"/>
+    <col min="5" max="5" width="38.59765625" customWidth="1"/>
+    <col min="6" max="6" width="25.1328125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2281,7 +2128,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="90">
+    <row r="2" spans="1:7" ht="90.4" x14ac:dyDescent="0.45">
       <c r="A2" s="23" t="s">
         <v>7</v>
       </c>
@@ -2304,7 +2151,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="90">
+    <row r="3" spans="1:7" ht="90.4" x14ac:dyDescent="0.45">
       <c r="A3" s="23" t="s">
         <v>13</v>
       </c>
@@ -2327,7 +2174,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60">
+    <row r="4" spans="1:7" ht="60.4" x14ac:dyDescent="0.45">
       <c r="A4" s="23" t="s">
         <v>16</v>
       </c>
@@ -2348,7 +2195,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="75">
+    <row r="5" spans="1:7" ht="90.4" x14ac:dyDescent="0.45">
       <c r="A5" s="23" t="s">
         <v>19</v>
       </c>
@@ -2371,7 +2218,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="24" customFormat="1" ht="60">
+    <row r="6" spans="1:7" s="24" customFormat="1" ht="60.4" x14ac:dyDescent="0.45">
       <c r="A6" s="23" t="s">
         <v>24</v>
       </c>
@@ -2394,7 +2241,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="75">
+    <row r="7" spans="1:7" ht="75.400000000000006" x14ac:dyDescent="0.45">
       <c r="A7" s="23" t="s">
         <v>29</v>
       </c>
@@ -2417,7 +2264,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="90">
+    <row r="8" spans="1:7" ht="90.4" x14ac:dyDescent="0.45">
       <c r="A8" s="23" t="s">
         <v>33</v>
       </c>
@@ -2440,7 +2287,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="75">
+    <row r="9" spans="1:7" ht="90.4" x14ac:dyDescent="0.45">
       <c r="A9" s="23" t="s">
         <v>37</v>
       </c>
@@ -2461,7 +2308,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="26" customFormat="1">
+    <row r="10" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="25"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -2487,22 +2334,22 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="25.59765625" style="9" customWidth="1"/>
     <col min="2" max="2" width="28" style="21" customWidth="1"/>
-    <col min="3" max="3" width="47.625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="50.75" style="21" customWidth="1"/>
-    <col min="5" max="5" width="38.625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="25.125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="47.59765625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="50.73046875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="38.59765625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="25.1328125" style="9" customWidth="1"/>
     <col min="7" max="7" width="17" style="9" customWidth="1"/>
     <col min="8" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2525,7 +2372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="135">
+    <row r="2" spans="1:7" ht="150" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>40</v>
       </c>
@@ -2548,7 +2395,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="135">
+    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>40</v>
       </c>
@@ -2571,7 +2418,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="165">
+    <row r="4" spans="1:7" ht="180" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>49</v>
       </c>
@@ -2594,7 +2441,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="135">
+    <row r="5" spans="1:7" ht="150" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>49</v>
       </c>
@@ -2617,7 +2464,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="135">
+    <row r="6" spans="1:7" ht="150" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
         <v>55</v>
       </c>
@@ -2640,7 +2487,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="135">
+    <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.45">
       <c r="A7" s="19" t="s">
         <v>55</v>
       </c>
@@ -2663,7 +2510,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="135">
+    <row r="8" spans="1:7" ht="150" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
         <v>61</v>
       </c>
@@ -2686,7 +2533,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="135">
+    <row r="9" spans="1:7" ht="150" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
         <v>61</v>
       </c>
@@ -2709,7 +2556,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="135">
+    <row r="10" spans="1:7" ht="150" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
         <v>61</v>
       </c>
@@ -2732,7 +2579,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="135">
+    <row r="11" spans="1:7" ht="150" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
         <v>69</v>
       </c>
@@ -2755,7 +2602,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="135">
+    <row r="12" spans="1:7" ht="150" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
         <v>69</v>
       </c>
@@ -2778,7 +2625,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.45">
       <c r="A13" s="19" t="s">
         <v>75</v>
       </c>
@@ -2801,7 +2648,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="90">
+    <row r="14" spans="1:7" ht="105" x14ac:dyDescent="0.45">
       <c r="A14" s="19" t="s">
         <v>79</v>
       </c>
@@ -2838,24 +2685,24 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.625" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="47.625" customWidth="1"/>
-    <col min="4" max="4" width="50.75" customWidth="1"/>
-    <col min="5" max="5" width="38.625" customWidth="1"/>
-    <col min="6" max="6" width="25.125" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="1" max="1" width="47.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.59765625" customWidth="1"/>
+    <col min="6" max="6" width="52.59765625" style="27" customWidth="1"/>
+    <col min="7" max="7" width="23.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2871,332 +2718,171 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="99.75">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:7" s="9" customFormat="1" ht="120" x14ac:dyDescent="0.45">
+      <c r="A2" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="E2" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="G2" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="9" customFormat="1" ht="120" x14ac:dyDescent="0.45">
+      <c r="A3" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="E2" s="27" t="s">
-        <v>287</v>
-      </c>
-      <c r="F2" s="27" t="s">
+      <c r="B3" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="G2" s="28">
+      <c r="C3" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="G3" s="19">
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="99.75">
-      <c r="A3" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="B3" s="27" t="s">
+    <row r="4" spans="1:7" s="9" customFormat="1" ht="120" x14ac:dyDescent="0.45">
+      <c r="A4" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="B4" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="C4" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="G3" s="28">
+      <c r="E4" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="G4" s="19">
         <v>2024</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="85.5">
-      <c r="A4" s="27" t="s">
+    <row r="5" spans="1:7" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.45">
+      <c r="A5" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B5" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C5" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="E5" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="G5" s="19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="9" customFormat="1" ht="120" x14ac:dyDescent="0.45">
+      <c r="A6" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>289</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="G4" s="28">
+      <c r="B6" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" s="19">
         <v>2024</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="99.75">
-      <c r="A5" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="C5" s="27" t="s">
+    <row r="7" spans="1:7" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.45">
+      <c r="A7" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="B7" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="E5" s="27" t="s">
-        <v>284</v>
-      </c>
-      <c r="F5" s="27" t="s">
+      <c r="C7" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="G5" s="28">
+      <c r="E7" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G7" s="19">
         <v>2024</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="99.75">
-      <c r="A6" s="23" t="s">
+    <row r="8" spans="1:7" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.45">
+      <c r="A8" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B8" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C8" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="G6" s="20">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="71.25">
-      <c r="A7" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>247</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>248</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="G7" s="20">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="75">
-      <c r="A8" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="B8" s="23" t="s">
+      <c r="E8" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>252</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>253</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>291</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="G8" s="20">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="105">
-      <c r="A9" s="23" t="s">
-        <v>254</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>255</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>256</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>257</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="G9" s="20">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="45">
-      <c r="A10" s="23" t="s">
-        <v>258</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>259</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="D10" s="23" t="s">
+      <c r="F8" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="E10" s="27" t="s">
-        <v>262</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="G10" s="20">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="45">
-      <c r="A11" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>282</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>265</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="G11" s="20">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="45">
-      <c r="A12" s="23" t="s">
-        <v>267</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>268</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>286</v>
-      </c>
-      <c r="F12" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="G12" s="20">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="75">
-      <c r="A13" s="23" t="s">
-        <v>269</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>270</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>271</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>272</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>293</v>
-      </c>
-      <c r="F13" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="G13" s="20">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45">
-      <c r="A14" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>274</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>275</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>276</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>294</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="G14" s="20">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="105">
-      <c r="A15" s="23" t="s">
-        <v>277</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>278</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>279</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>280</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>295</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>281</v>
-      </c>
-      <c r="G15" s="20">
+      <c r="G8" s="19">
         <v>2024</v>
       </c>
     </row>
@@ -3220,19 +2906,19 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="25.59765625" style="9" customWidth="1"/>
     <col min="2" max="2" width="28" style="9" customWidth="1"/>
-    <col min="3" max="3" width="47.625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="50.75" style="9" customWidth="1"/>
-    <col min="5" max="5" width="38.625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="25.125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="47.59765625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="50.73046875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="38.59765625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="25.1328125" style="9" customWidth="1"/>
     <col min="7" max="7" width="17" style="9" customWidth="1"/>
     <col min="8" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3255,7 +2941,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="90">
+    <row r="2" spans="1:7" ht="105" x14ac:dyDescent="0.45">
       <c r="A2" s="17" t="s">
         <v>86</v>
       </c>
@@ -3278,7 +2964,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="75">
+    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.45">
       <c r="A3" s="16" t="s">
         <v>93</v>
       </c>
@@ -3301,7 +2987,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="90">
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.45">
       <c r="A4" s="17" t="s">
         <v>98</v>
       </c>
@@ -3324,7 +3010,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="75">
+    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.45">
       <c r="A5" s="16" t="s">
         <v>86</v>
       </c>
@@ -3347,7 +3033,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="75">
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.45">
       <c r="A6" s="17" t="s">
         <v>93</v>
       </c>
@@ -3370,7 +3056,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="90">
+    <row r="7" spans="1:7" ht="90" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>98</v>
       </c>
@@ -3393,7 +3079,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="270">
+    <row r="8" spans="1:7" ht="285" x14ac:dyDescent="0.45">
       <c r="A8" s="17" t="s">
         <v>112</v>
       </c>
@@ -3416,7 +3102,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="60">
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>119</v>
       </c>
@@ -3439,7 +3125,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60">
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.45">
       <c r="A10" s="17" t="s">
         <v>125</v>
       </c>
@@ -3462,7 +3148,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="120">
+    <row r="11" spans="1:7" ht="135" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>131</v>
       </c>
@@ -3485,7 +3171,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="105">
+    <row r="12" spans="1:7" ht="120" x14ac:dyDescent="0.45">
       <c r="A12" s="17" t="s">
         <v>136</v>
       </c>
@@ -3508,7 +3194,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="75">
+    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.45">
       <c r="A13" s="16" t="s">
         <v>142</v>
       </c>
@@ -3531,7 +3217,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="75">
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.45">
       <c r="A14" s="17" t="s">
         <v>147</v>
       </c>
@@ -3554,7 +3240,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="195">
+    <row r="15" spans="1:7" ht="195" x14ac:dyDescent="0.45">
       <c r="A15" s="16" t="s">
         <v>151</v>
       </c>
@@ -3577,7 +3263,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="135">
+    <row r="16" spans="1:7" ht="135" x14ac:dyDescent="0.45">
       <c r="A16" s="17" t="s">
         <v>157</v>
       </c>
@@ -3600,7 +3286,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="135">
+    <row r="17" spans="1:7" ht="135" x14ac:dyDescent="0.45">
       <c r="A17" s="16" t="s">
         <v>157</v>
       </c>
@@ -3623,7 +3309,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="90">
+    <row r="18" spans="1:7" ht="105" x14ac:dyDescent="0.45">
       <c r="A18" s="17" t="s">
         <v>166</v>
       </c>
@@ -3646,7 +3332,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="90">
+    <row r="19" spans="1:7" ht="105" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
         <v>171</v>
       </c>
@@ -3667,7 +3353,7 @@
       </c>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:7" ht="90">
+    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.45">
       <c r="A20" s="17" t="s">
         <v>177</v>
       </c>
@@ -3690,7 +3376,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="90">
+    <row r="21" spans="1:7" ht="105" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
         <v>183</v>
       </c>
@@ -3713,7 +3399,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="75">
+    <row r="22" spans="1:7" ht="90" x14ac:dyDescent="0.45">
       <c r="A22" s="17" t="s">
         <v>189</v>
       </c>
@@ -3754,18 +3440,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.625" customWidth="1"/>
+    <col min="1" max="1" width="25.59765625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="47.625" customWidth="1"/>
-    <col min="4" max="4" width="50.75" customWidth="1"/>
-    <col min="5" max="5" width="38.625" customWidth="1"/>
-    <col min="6" max="6" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="47.59765625" customWidth="1"/>
+    <col min="4" max="4" width="50.73046875" customWidth="1"/>
+    <col min="5" max="5" width="38.59765625" customWidth="1"/>
+    <col min="6" max="6" width="25.1328125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3788,7 +3474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="90">
+    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>194</v>
       </c>
@@ -3811,7 +3497,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="60">
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>199</v>
       </c>
@@ -3834,7 +3520,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60">
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>204</v>
       </c>
@@ -3857,7 +3543,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="75">
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>209</v>
       </c>
@@ -3880,7 +3566,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="90">
+    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>214</v>
       </c>
@@ -3903,7 +3589,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="75">
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>220</v>
       </c>
@@ -3936,6 +3622,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bd2b4508-43bb-43a9-949a-527d9edee5a0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006395861A52F15448BD3944CBD4C58617" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee4bdd7030f0ea7859f0af66fe99e547">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bd2b4508-43bb-43a9-949a-527d9edee5a0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="719c67f33cf9376c21946e0c443abf4c" ns3:_="">
     <xsd:import namespace="bd2b4508-43bb-43a9-949a-527d9edee5a0"/>
@@ -4123,24 +3826,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1ADD084-BC56-46F9-993B-1BFE8BDA123B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bd2b4508-43bb-43a9-949a-527d9edee5a0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bd2b4508-43bb-43a9-949a-527d9edee5a0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0753EEC0-270F-4C9C-9E87-6EB2D8E16582}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D656A5-8B52-4FDF-93EC-791B5E719C59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4156,22 +3860,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0753EEC0-270F-4C9C-9E87-6EB2D8E16582}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1ADD084-BC56-46F9-993B-1BFE8BDA123B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bd2b4508-43bb-43a9-949a-527d9edee5a0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>